<commit_message>
Updated agenda and retro
</commit_message>
<xml_diff>
--- a/src/tools/Coding Agenda TTS.xlsx
+++ b/src/tools/Coding Agenda TTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\Projects\calendargroup\src\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\Sound recordings\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1987105B-E75F-4B3F-B69F-59051FF3D355}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE49FD7-3593-4340-AD17-1F789E9F6E23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="18240" windowHeight="12000" xr2:uid="{3178B449-25BE-475A-A714-010F31B586E6}"/>
+    <workbookView xWindow="6024" yWindow="0" windowWidth="14136" windowHeight="12000" xr2:uid="{3178B449-25BE-475A-A714-010F31B586E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Done</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Time to Code</t>
   </si>
   <si>
-    <t>Time for Retro</t>
-  </si>
-  <si>
     <t>Time for Break</t>
   </si>
   <si>
@@ -52,6 +49,12 @@
   </si>
   <si>
     <t>echo . . .</t>
+  </si>
+  <si>
+    <t>Time to Code with Red Green Refactor; do full cycles of TDD</t>
+  </si>
+  <si>
+    <t>Time for Retro and Red Green Refactor Start Time Verification</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E30"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,7 +458,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -480,7 +483,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" t="str">
-        <f t="shared" ref="E5:E30" si="1">IF(C4=0,"echo :-)","timeout %_"&amp;C4&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E5" si="1">IF(C4=0,"echo :-)","timeout %_"&amp;C4&amp;"MinuteTimeout%")</f>
         <v>timeout %_10MinuteTimeout%</v>
       </c>
     </row>
@@ -489,7 +492,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -498,7 +501,7 @@
         <v>0.40624999999999994</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -506,7 +509,7 @@
       <c r="D7" s="2"/>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>call:speak "Time to Code for 25 minutes"</v>
+        <v>call:speak "Time to Code with Red Green Refactor; do full cycles of TDD for 25 minutes"</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -514,7 +517,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" t="str">
-        <f t="shared" ref="E8:E30" si="2">IF(C7=0,"echo :-)","timeout %_"&amp;C7&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E8" si="2">IF(C7=0,"echo :-)","timeout %_"&amp;C7&amp;"MinuteTimeout%")</f>
         <v>timeout %_25MinuteTimeout%</v>
       </c>
     </row>
@@ -523,7 +526,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -532,7 +535,7 @@
         <v>0.42361111111111105</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -540,7 +543,7 @@
       <c r="D10" s="2"/>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>call:speak "Time for Retro for 5 minutes"</v>
+        <v>call:speak "Time for Retro and Red Green Refactor Start Time Verification for 5 minutes"</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -548,7 +551,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" t="str">
-        <f t="shared" ref="E11:E30" si="3">IF(C10=0,"echo :-)","timeout %_"&amp;C10&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E11" si="3">IF(C10=0,"echo :-)","timeout %_"&amp;C10&amp;"MinuteTimeout%")</f>
         <v>timeout %_5MinuteTimeout%</v>
       </c>
     </row>
@@ -557,7 +560,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -582,7 +585,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" t="str">
-        <f t="shared" ref="E14:E30" si="4">IF(C13=0,"echo :-)","timeout %_"&amp;C13&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E14" si="4">IF(C13=0,"echo :-)","timeout %_"&amp;C13&amp;"MinuteTimeout%")</f>
         <v>timeout %_15MinuteTimeout%</v>
       </c>
     </row>
@@ -591,7 +594,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -600,7 +603,7 @@
         <v>0.43749999999999994</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1">
         <v>10</v>
@@ -616,7 +619,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" t="str">
-        <f t="shared" ref="E17:E30" si="5">IF(C16=0,"echo :-)","timeout %_"&amp;C16&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E17" si="5">IF(C16=0,"echo :-)","timeout %_"&amp;C16&amp;"MinuteTimeout%")</f>
         <v>timeout %_10MinuteTimeout%</v>
       </c>
     </row>
@@ -625,7 +628,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -650,7 +653,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" t="str">
-        <f t="shared" ref="E20:E30" si="6">IF(C19=0,"echo :-)","timeout %_"&amp;C19&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E20" si="6">IF(C19=0,"echo :-)","timeout %_"&amp;C19&amp;"MinuteTimeout%")</f>
         <v>timeout %_30MinuteTimeout%</v>
       </c>
     </row>
@@ -659,7 +662,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -668,7 +671,7 @@
         <v>0.46527777777777768</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1">
         <v>15</v>
@@ -684,7 +687,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" t="str">
-        <f t="shared" ref="E23:E30" si="7">IF(C22=0,"echo :-)","timeout %_"&amp;C22&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E23" si="7">IF(C22=0,"echo :-)","timeout %_"&amp;C22&amp;"MinuteTimeout%")</f>
         <v>timeout %_15MinuteTimeout%</v>
       </c>
     </row>
@@ -693,7 +696,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -702,7 +705,7 @@
         <v>0.47569444444444436</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
         <v>5</v>
@@ -715,13 +718,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E26" t="str">
-        <f t="shared" ref="E26:E30" si="8">IF(C25=0,"echo :-)","timeout %_"&amp;C25&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E26" si="8">IF(C25=0,"echo :-)","timeout %_"&amp;C25&amp;"MinuteTimeout%")</f>
         <v>timeout %_5MinuteTimeout%</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -742,13 +745,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E29" t="str">
-        <f t="shared" ref="E29:E30" si="9">IF(C28=0,"echo :-)","timeout %_"&amp;C28&amp;"MinuteTimeout%")</f>
+        <f t="shared" ref="E29" si="9">IF(C28=0,"echo :-)","timeout %_"&amp;C28&amp;"MinuteTimeout%")</f>
         <v>echo :-)</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>